<commit_message>
added 2nd qoute for testing random pull
</commit_message>
<xml_diff>
--- a/01_Data/awesome_quotes.xlsx
+++ b/01_Data/awesome_quotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdexter/Desktop/auto_quotes/01_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9D7D29-F335-ED42-B2B1-3150C717507D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE5EF52-44F4-D347-9650-845DFEF3317A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>topic</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Be the person with embarrassing goals and impressive results instead of one of the many people with impressive goals and embarrassing results.</t>
+  </si>
+  <si>
+    <t>Repetition of the same thought or physical action develops into a habit which, repeated frequently enough, becomes an automatic reflex.</t>
+  </si>
+  <si>
+    <t>Norman Vincent Peale</t>
   </si>
 </sst>
 </file>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,6 +474,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
added quote to table
</commit_message>
<xml_diff>
--- a/01_Data/awesome_quotes.xlsx
+++ b/01_Data/awesome_quotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdexter/Desktop/auto_quotes/01_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE5EF52-44F4-D347-9650-845DFEF3317A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED7CFCB-7B1B-DC4C-93BD-3A45FEFE3E52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-10340" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>topic</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Norman Vincent Peale</t>
+  </si>
+  <si>
+    <t>The chains of habit are too weak to be felt until they are too strong to be broken.</t>
+  </si>
+  <si>
+    <t>Samuel Johnson</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,6 +491,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
added another quote to data-table
</commit_message>
<xml_diff>
--- a/01_Data/awesome_quotes.xlsx
+++ b/01_Data/awesome_quotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdexter/Desktop/auto_quotes/01_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED7CFCB-7B1B-DC4C-93BD-3A45FEFE3E52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15838DA9-8B5A-804E-ABD9-9FA3AF911DBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-10340" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>topic</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Samuel Johnson</t>
+  </si>
+  <si>
+    <t>Really successful people feel the same lack of motivation as everyone else.  The difference is that they still find a way to show up despite the feelings of boredom.</t>
+  </si>
+  <si>
+    <t>James Clear</t>
+  </si>
+  <si>
+    <t>Goals are good for setting a direction, but systems are best for making progress.</t>
+  </si>
+  <si>
+    <t>systems</t>
   </si>
 </sst>
 </file>
@@ -446,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,6 +514,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
added more quotes to data-table
</commit_message>
<xml_diff>
--- a/01_Data/awesome_quotes.xlsx
+++ b/01_Data/awesome_quotes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdexter/Desktop/auto_quotes/01_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdexter/Desktop/auto_quotes/01_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15838DA9-8B5A-804E-ABD9-9FA3AF911DBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2346AA35-7E4F-8542-8C1B-B501D77980A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-10340" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>topic</t>
   </si>
@@ -67,6 +67,30 @@
   </si>
   <si>
     <t>systems</t>
+  </si>
+  <si>
+    <t>You do not rise to the level of your goals. You fall to the level of your systems.</t>
+  </si>
+  <si>
+    <t>If you want better results, then forget about setting goals. Focus on your system instead.</t>
+  </si>
+  <si>
+    <t>With outcome-based habits, the focus is on what you want to achieve. With identity-based habits, the focus is on who you wish to become.</t>
+  </si>
+  <si>
+    <t>Motivation is what gets you started. Habit is what keeps you going.</t>
+  </si>
+  <si>
+    <t>Jim Ryun</t>
+  </si>
+  <si>
+    <t>It's not what we do once in a while that shapes our lives. It's what we do consistently.</t>
+  </si>
+  <si>
+    <t>Anthony Robbins</t>
+  </si>
+  <si>
+    <t>consistency</t>
   </si>
 </sst>
 </file>
@@ -458,16 +482,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="86.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="128.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -534,6 +558,61 @@
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>